<commit_message>
updated table so it's better
</commit_message>
<xml_diff>
--- a/Paper Work/What information will be stored.xlsx
+++ b/Paper Work/What information will be stored.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Drive" sheetId="1" r:id="rId1"/>
     <sheet name="Recordset" sheetId="2" r:id="rId2"/>
-    <sheet name="Backup" sheetId="3" r:id="rId3"/>
+    <sheet name="Backups" sheetId="3" r:id="rId3"/>
     <sheet name="User Properties" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="68">
   <si>
     <t>Field Name</t>
   </si>
@@ -49,9 +49,6 @@
     <t>Drive Name</t>
   </si>
   <si>
-    <t>Drive_Name</t>
-  </si>
-  <si>
     <t>Stores the name of the removable drive</t>
   </si>
   <si>
@@ -224,15 +221,6 @@
   </si>
   <si>
     <t>INTEGER</t>
-  </si>
-  <si>
-    <t>Run on startup</t>
-  </si>
-  <si>
-    <t>startup</t>
-  </si>
-  <si>
-    <t>Will the program run on startup?</t>
   </si>
 </sst>
 </file>
@@ -580,7 +568,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -630,61 +618,61 @@
         <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -751,17 +739,17 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -769,99 +757,99 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" s="2">
         <v>0</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -910,70 +898,70 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -987,7 +975,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C18" sqref="C17:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1000,62 +988,54 @@
   <sheetData>
     <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>71</v>
-      </c>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>